<commit_message>
Update Lista de Chequeo Informe Final según Criterios ABET DB1.xlsx
</commit_message>
<xml_diff>
--- a/academics/DB1/Lista de Chequeo Informe Final según Criterios ABET DB1.xlsx
+++ b/academics/DB1/Lista de Chequeo Informe Final según Criterios ABET DB1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\oicampo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UAO\oicampo-uao.github.io\academics\DB1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4963AF16-9C9C-4092-B46E-D892BFC862B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="8520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -552,7 +553,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -723,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -756,9 +757,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -806,19 +804,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,7 +819,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1142,14 +1130,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -1186,35 +1174,35 @@
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35" t="s">
+      <c r="N3" s="30"/>
+      <c r="O3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35" t="s">
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1231,46 +1219,46 @@
       <c r="D4" s="12">
         <v>4</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>3</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="13">
-        <v>4</v>
-      </c>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="12">
+        <v>4</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="13">
-        <v>4</v>
-      </c>
-      <c r="M4" s="13" t="s">
+      <c r="L4" s="12">
+        <v>4</v>
+      </c>
+      <c r="M4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="12">
         <v>5</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="12">
         <v>5</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="37">
+      <c r="R4" s="32">
         <v>5</v>
       </c>
       <c r="S4" s="7">
@@ -1282,38 +1270,38 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>0</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="31">
         <v>1</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31">
         <v>1</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36">
+      <c r="F5" s="31"/>
+      <c r="G5" s="31">
         <v>1</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36">
+      <c r="H5" s="31"/>
+      <c r="I5" s="31">
         <v>1</v>
       </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36">
+      <c r="J5" s="31"/>
+      <c r="K5" s="31">
         <v>1</v>
       </c>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36">
+      <c r="L5" s="31"/>
+      <c r="M5" s="31">
         <v>1</v>
       </c>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36">
+      <c r="N5" s="31"/>
+      <c r="O5" s="31">
         <v>1</v>
       </c>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36">
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31">
         <v>1</v>
       </c>
     </row>
@@ -1321,1134 +1309,1134 @@
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="17" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:19" s="16" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>0.08</v>
       </c>
-      <c r="C7" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="26">
+      <c r="C7" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="25">
         <f>C7*5</f>
         <v>4</v>
       </c>
-      <c r="E7" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="F7" s="16">
+      <c r="E7" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="15">
         <f>E7*5</f>
         <v>4.5</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>0.7</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <f>G7*5</f>
         <v>3.5</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <v>1</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <f>I7*5</f>
         <v>5</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <v>0.7</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <f>K7*5</f>
         <v>3.5</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <v>0.87</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="25">
         <f>M7*5</f>
         <v>4.3499999999999996</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="15">
         <v>0.5</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="25">
         <f>O7*5</f>
         <v>2.5</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="15">
         <v>0.7</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="25">
         <f>Q7*5</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="34" customFormat="1" ht="72.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:19" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>0.04</v>
       </c>
-      <c r="C8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="D8" s="33">
+      <c r="C8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="14">
         <f t="shared" ref="D8:D23" si="0">C8*5</f>
         <v>4.5</v>
       </c>
-      <c r="E8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="F8" s="32">
+      <c r="E8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="F8" s="13">
         <f t="shared" ref="F8:F23" si="1">E8*5</f>
         <v>4.5</v>
       </c>
-      <c r="G8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="H8" s="32">
+      <c r="G8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="13">
         <f t="shared" ref="H8:H23" si="2">G8*5</f>
         <v>4.5</v>
       </c>
-      <c r="I8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="J8" s="33">
+      <c r="I8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="J8" s="14">
         <f t="shared" ref="J8:J23" si="3">I8*5</f>
         <v>4.5</v>
       </c>
-      <c r="K8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="L8" s="33">
+      <c r="K8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="L8" s="14">
         <f t="shared" ref="L8:L23" si="4">K8*5</f>
         <v>4.5</v>
       </c>
-      <c r="M8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="N8" s="33">
+      <c r="M8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="14">
         <f t="shared" ref="N8:N23" si="5">M8*5</f>
         <v>4.5</v>
       </c>
-      <c r="O8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="P8" s="33">
+      <c r="O8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="P8" s="14">
         <f t="shared" ref="P8:P23" si="6">O8*5</f>
         <v>4.5</v>
       </c>
-      <c r="Q8" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="R8" s="33">
+      <c r="Q8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="R8" s="14">
         <f t="shared" ref="R8:R23" si="7">Q8*5</f>
         <v>4.5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="34" customFormat="1" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:19" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>0.04</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="13">
         <v>0.85</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="13">
         <v>0.85</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="13">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="13">
         <v>0.85</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="13">
         <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="13">
         <v>0.85</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="14">
         <f t="shared" si="3"/>
         <v>4.25</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="13">
         <v>0.85</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="14">
         <f t="shared" si="4"/>
         <v>4.25</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="13">
         <v>0.85</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="14">
         <f t="shared" si="5"/>
         <v>4.25</v>
       </c>
-      <c r="O9" s="32">
+      <c r="O9" s="13">
         <v>0.85</v>
       </c>
-      <c r="P9" s="33">
+      <c r="P9" s="14">
         <f t="shared" si="6"/>
         <v>4.25</v>
       </c>
-      <c r="Q9" s="32">
+      <c r="Q9" s="13">
         <v>0.85</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="14">
         <f t="shared" si="7"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="34" customFormat="1" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:19" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>0.04</v>
       </c>
-      <c r="C10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="D10" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="F10" s="32">
+      <c r="E10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="13">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="H10" s="32">
+      <c r="G10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="J10" s="33">
+      <c r="I10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="14">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="K10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="L10" s="33">
+      <c r="K10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L10" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="M10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="N10" s="33">
+      <c r="M10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="N10" s="14">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="P10" s="33">
+      <c r="O10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="P10" s="14">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q10" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="R10" s="33">
+      <c r="Q10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="R10" s="14">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="17" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:19" s="16" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>0.05</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>0.85</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="25">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="E11" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="F11" s="16">
+      <c r="E11" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F11" s="15">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <v>0.95</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <f t="shared" si="2"/>
         <v>4.75</v>
       </c>
-      <c r="I11" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="J11" s="26">
+      <c r="I11" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="25">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="K11" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="L11" s="26">
+      <c r="K11" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="L11" s="25">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="M11" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="N11" s="26">
+      <c r="M11" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="N11" s="25">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O11" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="P11" s="26">
+      <c r="O11" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P11" s="25">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q11" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="R11" s="26">
+      <c r="Q11" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="R11" s="25">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="17" customFormat="1" ht="243.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:19" s="16" customFormat="1" ht="243.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>0.1</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>0.85</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="25">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="E12" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="F12" s="16">
+      <c r="E12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F12" s="15">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <v>0.85</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
-      <c r="I12" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="J12" s="26">
+      <c r="I12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J12" s="25">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="K12" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="L12" s="26">
+      <c r="K12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="L12" s="25">
         <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
-      <c r="M12" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="N12" s="26">
+      <c r="M12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="N12" s="25">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="15">
         <v>0.85</v>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="25">
         <f t="shared" si="6"/>
         <v>4.25</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="15">
         <v>0.7</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="25">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="17" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:19" s="16" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>0.1</v>
       </c>
-      <c r="C13" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="C13" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="D13" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E13" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="F13" s="16">
+      <c r="E13" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F13" s="15">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <v>0.7</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="I13" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="J13" s="26">
+      <c r="I13" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J13" s="25">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="K13" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="L13" s="26">
+      <c r="K13" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="L13" s="25">
         <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
-      <c r="M13" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="N13" s="26">
+      <c r="M13" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="N13" s="25">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O13" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="P13" s="26">
+      <c r="O13" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P13" s="25">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="15">
         <v>0.6</v>
       </c>
-      <c r="R13" s="26">
+      <c r="R13" s="25">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="17" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:19" s="16" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>0.1</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>0.88</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="E14" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="F14" s="16">
+      <c r="E14" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F14" s="15">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="15">
         <v>0.85</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
-      <c r="I14" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="J14" s="26">
+      <c r="I14" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="J14" s="25">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="K14" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="L14" s="26">
+      <c r="K14" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="L14" s="25">
         <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
-      <c r="M14" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="N14" s="26">
+      <c r="M14" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="N14" s="25">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O14" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="P14" s="26">
+      <c r="O14" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P14" s="25">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="15">
         <v>0.7</v>
       </c>
-      <c r="R14" s="26">
+      <c r="R14" s="25">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="34" customFormat="1" ht="201" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:19" ht="215.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="29">
         <v>0.05</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="13">
         <v>0.85</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="14">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="E15" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="F15" s="32">
+      <c r="E15" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="F15" s="13">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="13">
         <v>0.85</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="13">
         <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="13">
         <v>0.85</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="14">
         <f t="shared" si="3"/>
         <v>4.25</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="13">
         <v>0.85</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="14">
         <f t="shared" si="4"/>
         <v>4.25</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="13">
         <v>0.87</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="14">
         <f t="shared" si="5"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="13">
         <v>0.85</v>
       </c>
-      <c r="P15" s="33">
+      <c r="P15" s="14">
         <f t="shared" si="6"/>
         <v>4.25</v>
       </c>
-      <c r="Q15" s="32">
+      <c r="Q15" s="13">
         <v>0.85</v>
       </c>
-      <c r="R15" s="33">
+      <c r="R15" s="14">
         <f t="shared" si="7"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="29" customFormat="1" ht="315" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="28" customFormat="1" ht="315" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>0.25</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>0.6</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="27">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E16" s="27">
-        <v>0.9</v>
-      </c>
-      <c r="F16" s="27">
+      <c r="E16" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="F16" s="26">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="26">
         <v>0.6</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="26">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <v>0.6</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="27">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="K16" s="27">
-        <v>0.9</v>
-      </c>
-      <c r="L16" s="28">
+      <c r="K16" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="L16" s="27">
         <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
-      <c r="M16" s="27">
-        <v>0.9</v>
-      </c>
-      <c r="N16" s="28">
+      <c r="M16" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="N16" s="27">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O16" s="27">
-        <v>0.8</v>
-      </c>
-      <c r="P16" s="28">
+      <c r="O16" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="P16" s="27">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q16" s="27">
+      <c r="Q16" s="26">
         <v>0.7</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="27">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="17" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:18" s="16" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="26">
+      <c r="B17" s="21"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16">
+      <c r="E17" s="15"/>
+      <c r="F17" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16">
+      <c r="G17" s="15"/>
+      <c r="H17" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="26">
+      <c r="I17" s="15"/>
+      <c r="J17" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="26">
+      <c r="K17" s="15"/>
+      <c r="L17" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="26">
+      <c r="M17" s="15"/>
+      <c r="N17" s="25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="26">
+      <c r="O17" s="15"/>
+      <c r="P17" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="26">
+      <c r="Q17" s="15"/>
+      <c r="R17" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="17" customFormat="1" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:18" s="16" customFormat="1" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>0.6</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="15">
         <v>0.5</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="15">
         <v>0.4</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="15">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="15">
         <v>0.5</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="25">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="15">
         <v>0.5</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="25">
         <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18" s="15">
         <v>1</v>
       </c>
-      <c r="N18" s="26">
+      <c r="N18" s="25">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="15">
         <v>0.4</v>
       </c>
-      <c r="P18" s="26">
+      <c r="P18" s="25">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18" s="15">
         <v>0.5</v>
       </c>
-      <c r="R18" s="26">
+      <c r="R18" s="25">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="17" customFormat="1" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:18" s="16" customFormat="1" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>0.85</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="25">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>0.85</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="15">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
-      <c r="G19" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="H19" s="16">
+      <c r="G19" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="H19" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I19" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="J19" s="26">
+      <c r="I19" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="J19" s="25">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="15">
         <v>0.7</v>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="25">
         <f t="shared" si="4"/>
         <v>3.5</v>
       </c>
-      <c r="M19" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="N19" s="26">
+      <c r="M19" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="N19" s="25">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="15">
         <v>0.7</v>
       </c>
-      <c r="P19" s="26">
+      <c r="P19" s="25">
         <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="15">
         <v>0.5</v>
       </c>
-      <c r="R19" s="26">
+      <c r="R19" s="25">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>0.87</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="25">
         <f t="shared" si="0"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>0.87</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="15">
         <f t="shared" si="1"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="G20" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="H20" s="16">
+      <c r="G20" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="15">
         <v>0.85</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="25">
         <f t="shared" si="3"/>
         <v>4.25</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="15">
         <v>0.7</v>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="25">
         <f t="shared" si="4"/>
         <v>3.5</v>
       </c>
-      <c r="M20" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="N20" s="26">
+      <c r="M20" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="N20" s="25">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="15">
         <v>0.7</v>
       </c>
-      <c r="P20" s="26">
+      <c r="P20" s="25">
         <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20" s="15">
         <v>0.5</v>
       </c>
-      <c r="R20" s="26">
+      <c r="R20" s="25">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <v>0.88</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="25">
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>0.88</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="G21" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="H21" s="16">
+      <c r="G21" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I21" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="J21" s="26">
+      <c r="I21" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="25">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="15">
         <v>0.7</v>
       </c>
-      <c r="L21" s="26">
+      <c r="L21" s="25">
         <f t="shared" si="4"/>
         <v>3.5</v>
       </c>
-      <c r="M21" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="N21" s="26">
+      <c r="M21" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="N21" s="25">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="15">
         <v>0.7</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="25">
         <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="15">
         <v>0.7</v>
       </c>
-      <c r="R21" s="26">
+      <c r="R21" s="25">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="34" customFormat="1" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:18" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="29">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="D22" s="33">
+      <c r="C22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="D22" s="14">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="E22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="F22" s="32">
+      <c r="E22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="F22" s="13">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="G22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="H22" s="32">
+      <c r="G22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="H22" s="13">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
-      <c r="I22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="J22" s="33">
+      <c r="I22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="J22" s="14">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="K22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="L22" s="33">
+      <c r="K22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="L22" s="14">
         <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
-      <c r="M22" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="N22" s="33">
+      <c r="M22" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="N22" s="14">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="O22" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="P22" s="33">
+      <c r="O22" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="P22" s="14">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q22" s="32">
+      <c r="Q22" s="13">
         <v>0.85</v>
       </c>
-      <c r="R22" s="33">
+      <c r="R22" s="14">
         <f t="shared" si="7"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="34" customFormat="1" ht="72.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="29">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="13">
         <v>1</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="13">
         <v>1</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="13">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="13">
         <v>1</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="13">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="I23" s="32">
+      <c r="I23" s="13">
         <v>1</v>
       </c>
-      <c r="J23" s="33">
+      <c r="J23" s="14">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="K23" s="32">
+      <c r="K23" s="13">
         <v>1</v>
       </c>
-      <c r="L23" s="33">
+      <c r="L23" s="14">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="M23" s="32">
+      <c r="M23" s="13">
         <v>1</v>
       </c>
-      <c r="N23" s="33">
+      <c r="N23" s="14">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="13">
         <v>1</v>
       </c>
-      <c r="P23" s="33">
+      <c r="P23" s="14">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="Q23" s="32">
+      <c r="Q23" s="13">
         <v>1</v>
       </c>
-      <c r="R23" s="33">
+      <c r="R23" s="14">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="25">
+      <c r="B24" s="24">
         <f>SUM(B5:B23)</f>
         <v>1</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <f>5*(C5*$B$5+C7*$B$7+C8*$B$8+C9*$B$9+C10*$B$10+C11*$B$11+C12*$B$12+C13*$B$13+C14*$B$14+C15*$B$15+C16*$B$16+C18*$B$18+C19*$B$19+C20*$B$20+C21*$B$21+C22*$B$22+C23*$B$23)</f>
         <v>3.9075000000000011</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15">
+      <c r="D24" s="14"/>
+      <c r="E24" s="14">
         <f>5*(E5*$B$5+E7*$B$7+E8*$B$8+E9*$B$9+E10*$B$10+E11*$B$11+E12*$B$12+E13*$B$13+E14*$B$14+E15*$B$15+E16*$B$16+E18*$B$18+E19*$B$19+E20*$B$20+E21*$B$21+E22*$B$22+E23*$B$23)</f>
         <v>4.4200000000000008</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14">
         <f t="shared" ref="G24:M24" si="8">5*(G5*$B$5+G7*$B$7+G8*$B$8+G9*$B$9+G10*$B$10+G11*$B$11+G12*$B$12+G13*$B$13+G14*$B$14+G15*$B$15+G16*$B$16+G18*$B$18+G19*$B$19+G20*$B$20+G21*$B$21+G22*$B$22+G23*$B$23)</f>
         <v>3.7775000000000003</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15">
+      <c r="H24" s="14"/>
+      <c r="I24" s="14">
         <f t="shared" si="8"/>
         <v>4.0037500000000001</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15">
+      <c r="J24" s="14"/>
+      <c r="K24" s="14">
         <f t="shared" si="8"/>
         <v>4.2399999999999993</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15">
+      <c r="L24" s="14"/>
+      <c r="M24" s="14">
         <f t="shared" si="8"/>
         <v>4.4380000000000006</v>
       </c>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15">
+      <c r="N24" s="14"/>
+      <c r="O24" s="14">
         <f t="shared" ref="O24" si="9">5*(O5*$B$5+O7*$B$7+O8*$B$8+O9*$B$9+O10*$B$10+O11*$B$11+O12*$B$12+O13*$B$13+O14*$B$14+O15*$B$15+O16*$B$16+O18*$B$18+O19*$B$19+O20*$B$20+O21*$B$21+O22*$B$22+O23*$B$23)</f>
         <v>3.8849999999999998</v>
       </c>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15">
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14">
         <f t="shared" ref="Q24" si="10">5*(Q5*$B$5+Q7*$B$7+Q8*$B$8+Q9*$B$9+Q10*$B$10+Q11*$B$11+Q12*$B$12+Q13*$B$13+Q14*$B$14+Q15*$B$15+Q16*$B$16+Q18*$B$18+Q19*$B$19+Q20*$B$20+Q21*$B$21+Q22*$B$22+Q23*$B$23)</f>
         <v>3.5837499999999989</v>
       </c>

</xml_diff>